<commit_message>
add 1 code clinics - 20230808
</commit_message>
<xml_diff>
--- a/uploads/(Formatted)-20230807 Clinics - VN - Latest.xlsx
+++ b/uploads/(Formatted)-20230807 Clinics - VN - Latest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michace/Desktop/SAS/tools/sas-export-clinics-from-excel/uploads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{364C3CBE-E66C-0A4A-A698-C6C66E4D1C16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBA7490F-37AD-F044-8A97-3E851A22A5D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20260" xr2:uid="{CD5FCDE9-40CA-A645-8A7E-D71150EC814D}"/>
+    <workbookView xWindow="0" yWindow="840" windowWidth="34560" windowHeight="20260" xr2:uid="{CD5FCDE9-40CA-A645-8A7E-D71150EC814D}"/>
   </bookViews>
   <sheets>
     <sheet name="ALL" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7570" uniqueCount="3634">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7590" uniqueCount="3644">
   <si>
     <t>Tiếng Việt</t>
   </si>
@@ -11104,6 +11104,36 @@
   </si>
   <si>
     <t>45 Thanh Thai, Ward 4 District 10 Ho Chi Minh</t>
+  </si>
+  <si>
+    <t>NKXPLVS</t>
+  </si>
+  <si>
+    <t>474 Đ. Lê Văn Sỹ, Phường 14</t>
+  </si>
+  <si>
+    <t>028 3931 9191</t>
+  </si>
+  <si>
+    <t>Thứ 2 - CN: 08:00 - 17:00</t>
+  </si>
+  <si>
+    <t>Saint Paul Dental Clinic - Le Van Sy Branch</t>
+  </si>
+  <si>
+    <t>Ward 14</t>
+  </si>
+  <si>
+    <t>http://www.nhakhoasaintpaul.com/</t>
+  </si>
+  <si>
+    <t>474 Đ. Lê Văn Sỹ, Phường 14 Quận 3 Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>474 Le Van Sy street, Ward 14 District 3 Ho Chi Minh</t>
+  </si>
+  <si>
+    <t>Nha Khoa Saint Paul - CN Lê Văn Sỹ</t>
   </si>
 </sst>
 </file>
@@ -11543,7 +11573,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="153">
+  <cellXfs count="154">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -11966,6 +11996,9 @@
     </xf>
     <xf numFmtId="49" fontId="22" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -13024,10 +13057,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3996FE01-6E8E-7E4B-AF8A-2F606D870DA8}">
-  <dimension ref="A1:AE297"/>
+  <dimension ref="A1:AE298"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A277" zoomScale="94" workbookViewId="0">
-      <selection activeCell="C298" sqref="C298"/>
+    <sheetView tabSelected="1" topLeftCell="A279" zoomScale="94" workbookViewId="0">
+      <selection activeCell="AA300" sqref="AA300"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13072,36 +13105,36 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="4"/>
-      <c r="J1" s="145" t="s">
+      <c r="J1" s="146" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="145"/>
-      <c r="L1" s="145"/>
-      <c r="M1" s="145"/>
-      <c r="N1" s="145"/>
-      <c r="O1" s="145"/>
-      <c r="P1" s="145"/>
+      <c r="K1" s="146"/>
+      <c r="L1" s="146"/>
+      <c r="M1" s="146"/>
+      <c r="N1" s="146"/>
+      <c r="O1" s="146"/>
+      <c r="P1" s="146"/>
       <c r="Q1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="R1" s="146" t="s">
+      <c r="R1" s="147" t="s">
         <v>3</v>
       </c>
-      <c r="S1" s="146"/>
-      <c r="T1" s="146"/>
-      <c r="U1" s="147" t="s">
+      <c r="S1" s="147"/>
+      <c r="T1" s="147"/>
+      <c r="U1" s="148" t="s">
         <v>4</v>
       </c>
-      <c r="V1" s="147"/>
-      <c r="W1" s="148" t="s">
+      <c r="V1" s="148"/>
+      <c r="W1" s="149" t="s">
         <v>5</v>
       </c>
-      <c r="X1" s="149"/>
-      <c r="Y1" s="150"/>
-      <c r="Z1" s="151" t="s">
+      <c r="X1" s="150"/>
+      <c r="Y1" s="151"/>
+      <c r="Z1" s="152" t="s">
         <v>6</v>
       </c>
-      <c r="AA1" s="152"/>
+      <c r="AA1" s="153"/>
     </row>
     <row r="2" spans="1:29" ht="154" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
@@ -37746,6 +37779,81 @@
         <v>56</v>
       </c>
       <c r="AC297" s="115" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="298" spans="1:29" ht="17" x14ac:dyDescent="0.2">
+      <c r="A298" s="118" t="s">
+        <v>3634</v>
+      </c>
+      <c r="B298" s="126" t="s">
+        <v>1053</v>
+      </c>
+      <c r="C298" s="80" t="s">
+        <v>3643</v>
+      </c>
+      <c r="D298" s="127" t="s">
+        <v>3635</v>
+      </c>
+      <c r="E298" s="128" t="s">
+        <v>1705</v>
+      </c>
+      <c r="F298" s="129" t="s">
+        <v>3636</v>
+      </c>
+      <c r="G298" s="130" t="s">
+        <v>3637</v>
+      </c>
+      <c r="H298" s="145"/>
+      <c r="I298" s="131" t="s">
+        <v>43</v>
+      </c>
+      <c r="J298" s="83" t="s">
+        <v>3638</v>
+      </c>
+      <c r="K298" s="130" t="s">
+        <v>3639</v>
+      </c>
+      <c r="L298" s="132" t="s">
+        <v>1708</v>
+      </c>
+      <c r="M298" s="133" t="s">
+        <v>3636</v>
+      </c>
+      <c r="N298" s="130" t="s">
+        <v>1102</v>
+      </c>
+      <c r="O298" s="134"/>
+      <c r="P298" s="131" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q298" s="135" t="s">
+        <v>3640</v>
+      </c>
+      <c r="R298" s="125" t="s">
+        <v>51</v>
+      </c>
+      <c r="S298" s="125"/>
+      <c r="T298" s="125"/>
+      <c r="U298" s="125"/>
+      <c r="V298" s="125"/>
+      <c r="W298" s="28">
+        <v>10.78950818</v>
+      </c>
+      <c r="X298" s="28">
+        <v>106.6754595</v>
+      </c>
+      <c r="Y298" s="28"/>
+      <c r="Z298" t="s">
+        <v>3641</v>
+      </c>
+      <c r="AA298" t="s">
+        <v>3642</v>
+      </c>
+      <c r="AB298" s="115" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC298" s="115" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>